<commit_message>
test set cell font passes
</commit_message>
<xml_diff>
--- a/Test Open Xml/testdata/testsetcellfont.xlsx
+++ b/Test Open Xml/testdata/testsetcellfont.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="CAN1" sheetId="1" r:id="Rb55ece6edd574384"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="CAN1" sheetId="1" r:id="R6b8ee38d842a4db5"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -10,25 +10,37 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:si>
-    <x:t>A041F27D-0425-412A-88B9-8A7BA9010D0C</x:t>
+    <x:t>5A69EC84-EF7D-4B3F-9E62-F3AB8008BA65</x:t>
   </x:si>
 </x:sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <x:styleSheet xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:fonts count="1">
+  <x:fonts count="2">
+    <x:font/>
     <x:font>
       <x:b val="1"/>
-      <x:i val="1"/>
       <x:u val="double"/>
       <x:sz val="18"/>
       <x:color rgb="0003B400"/>
       <x:name val="Calibri"/>
     </x:font>
   </x:fonts>
-  <x:cellXfs count="1">
-    <x:xf fontId="0" applyFont="1"/>
+  <x:fills count="2">
+    <x:fill>
+      <x:patternFill patternType="none"/>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="gray125"/>
+    </x:fill>
+  </x:fills>
+  <x:borders count="1">
+    <x:border/>
+  </x:borders>
+  <x:cellXfs count="2">
+    <x:xf/>
+    <x:xf fontId="1" applyFont="1"/>
   </x:cellXfs>
 </x:styleSheet>
 </file>
@@ -37,7 +49,7 @@
 <x:worksheet xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheetData>
     <x:row r="2">
-      <x:c r="B2" s="0" t="s">
+      <x:c r="B2" s="1" t="s">
         <x:v>0</x:v>
       </x:c>
     </x:row>

</xml_diff>